<commit_message>
Undated results to Hexaly 14
</commit_message>
<xml_diff>
--- a/hexaly_benchmarking_results/mip_n.xlsx
+++ b/hexaly_benchmarking_results/mip_n.xlsx
@@ -19,10 +19,7 @@
     <t>acc</t>
   </si>
   <si>
-    <t>T3_U2</t>
-  </si>
-  <si>
-    <t>T4_U3</t>
+    <t>T1_U1</t>
   </si>
   <si>
     <t>T2_U2</t>
@@ -31,16 +28,19 @@
     <t>T4_U2</t>
   </si>
   <si>
-    <t>T1_U1</t>
+    <t>T3_U3</t>
+  </si>
+  <si>
+    <t>T3_U2</t>
+  </si>
+  <si>
+    <t>T2_U3</t>
+  </si>
+  <si>
+    <t>T4_U3</t>
   </si>
   <si>
     <t>T5_U4</t>
-  </si>
-  <si>
-    <t>T3_U3</t>
-  </si>
-  <si>
-    <t>T2_U3</t>
   </si>
 </sst>
 </file>
@@ -476,19 +476,19 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -496,28 +496,28 @@
         <v>40</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -525,7 +525,7 @@
         <v>30</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -534,16 +534,16 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -583,28 +583,28 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -612,19 +612,19 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -641,19 +641,19 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -670,28 +670,28 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -699,28 +699,28 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -728,25 +728,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <v>3</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I12">
         <v>3</v>
@@ -757,25 +757,25 @@
         <v>9</v>
       </c>
       <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
         <v>9</v>
       </c>
-      <c r="C13">
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
         <v>6</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
       </c>
       <c r="I13">
         <v>3</v>
@@ -786,28 +786,28 @@
         <v>8</v>
       </c>
       <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
         <v>7</v>
       </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>6</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
       <c r="G14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -815,25 +815,25 @@
         <v>7</v>
       </c>
       <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
         <v>7</v>
       </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>6</v>
-      </c>
       <c r="F15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I15">
         <v>4</v>
@@ -844,28 +844,28 @@
         <v>6</v>
       </c>
       <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
         <v>7</v>
       </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16">
+      <c r="F16">
         <v>10</v>
       </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
       <c r="G16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I16">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -873,28 +873,28 @@
         <v>5</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
         <v>7</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>6</v>
       </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>9</v>
-      </c>
       <c r="I17">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -902,28 +902,28 @@
         <v>4</v>
       </c>
       <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>12</v>
+      </c>
+      <c r="F18">
         <v>10</v>
       </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
-      <c r="F18">
+      <c r="G18">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
         <v>6</v>
-      </c>
-      <c r="G18">
-        <v>6</v>
-      </c>
-      <c r="H18">
-        <v>12</v>
-      </c>
-      <c r="I18">
-        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -931,28 +931,28 @@
         <v>3</v>
       </c>
       <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="E19">
         <v>16</v>
       </c>
-      <c r="C19">
+      <c r="F19">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
         <v>8</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>17</v>
-      </c>
-      <c r="F19">
-        <v>8</v>
-      </c>
-      <c r="G19">
-        <v>8</v>
-      </c>
-      <c r="H19">
-        <v>14</v>
-      </c>
-      <c r="I19">
-        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -960,28 +960,28 @@
         <v>2</v>
       </c>
       <c r="B20">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20">
         <v>26</v>
       </c>
-      <c r="F20">
-        <v>9</v>
-      </c>
       <c r="G20">
+        <v>13</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
         <v>10</v>
-      </c>
-      <c r="H20">
-        <v>11</v>
-      </c>
-      <c r="I20">
-        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -989,28 +989,28 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
         <v>51</v>
       </c>
-      <c r="F21">
-        <v>15</v>
-      </c>
       <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
         <v>16</v>
-      </c>
-      <c r="H21">
-        <v>17</v>
-      </c>
-      <c r="I21">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>